<commit_message>
few changes in deals page
</commit_message>
<xml_diff>
--- a/target/classes/com/hubspot/qa/testdata/HubSpotTestData.xlsx
+++ b/target/classes/com/hubspot/qa/testdata/HubSpotTestData.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NaveenKhunteta/Documents/workspace/SeptPOMSeries/src/main/java/com/hubspot/qa/testdata/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="860" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15975" windowHeight="3945" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="deal" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>email</t>
   </si>
@@ -112,13 +107,43 @@
   </si>
   <si>
     <t>test6@gmail.com</t>
+  </si>
+  <si>
+    <t>Pipeline</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>DealName</t>
+  </si>
+  <si>
+    <t>DealStage</t>
+  </si>
+  <si>
+    <t>deal1</t>
+  </si>
+  <si>
+    <t>pipe1</t>
+  </si>
+  <si>
+    <t>Appointment Scheduled</t>
+  </si>
+  <si>
+    <t>deal2</t>
+  </si>
+  <si>
+    <t>pipe2</t>
+  </si>
+  <si>
+    <t>Qualified To Buy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -161,9 +186,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -221,7 +247,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -256,7 +282,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -433,27 +459,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -481,7 +507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -495,7 +521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -509,7 +535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -523,7 +549,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -537,7 +563,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -557,13 +583,61 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="3" max="3" width="20.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3">
+        <v>21000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>